<commit_message>
Add toggle actual cases vs rate
</commit_message>
<xml_diff>
--- a/refreshed_daily_cases.xlsx
+++ b/refreshed_daily_cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6660" tabRatio="728"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="728"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">UTLAs!$A$8:$X$159</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1112,12 +1112,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="??,??0"/>
     <numFmt numFmtId="165" formatCode="?,???,??0"/>
     <numFmt numFmtId="166" formatCode="???,??0"/>
     <numFmt numFmtId="167" formatCode="???,??0;;??,???\-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1244,13 +1245,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1318,7 +1320,8 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1329,7 +1332,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Comma" xfId="4" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1647,9 +1651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1698,7 +1700,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
@@ -2455,6 +2457,17 @@
         <v>33718</v>
       </c>
     </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="26">
+        <v>43924</v>
+      </c>
+      <c r="B73" s="27">
+        <v>4450</v>
+      </c>
+      <c r="C73" s="27">
+        <v>38168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2462,7 +2475,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -2512,13 +2525,13 @@
       <c r="C6" s="24"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
@@ -2944,6 +2957,31 @@
       <c r="G32" s="25">
         <v>30</v>
       </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
+        <v>43924</v>
+      </c>
+      <c r="B33" s="25">
+        <v>684</v>
+      </c>
+      <c r="C33" s="25">
+        <v>3605</v>
+      </c>
+      <c r="D33" s="25">
+        <v>3302</v>
+      </c>
+      <c r="E33" s="25">
+        <v>126</v>
+      </c>
+      <c r="F33" s="25">
+        <v>141</v>
+      </c>
+      <c r="G33" s="25">
+        <v>36</v>
+      </c>
+      <c r="H33" s="23"/>
+      <c r="I33" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2955,7 +2993,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA13"/>
+  <dimension ref="A1:AB13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
@@ -2969,46 +3007,46 @@
     <col min="3" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.7109375" customWidth="1"/>
     <col min="22" max="24" width="10.7109375" style="23" customWidth="1"/>
-    <col min="25" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>325</v>
       </c>
       <c r="B3" s="11"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>324</v>
       </c>
       <c r="B4" s="11"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>326</v>
       </c>
       <c r="B5" s="11"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>327</v>
       </c>
       <c r="B6" s="11"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -3090,8 +3128,11 @@
       <c r="AA8" s="3">
         <v>43923</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB8" s="3">
+        <v>43924</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
@@ -3173,8 +3214,11 @@
       <c r="AA9" s="8">
         <v>28221</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB9" s="29">
+        <v>31797</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>2</v>
       </c>
@@ -3254,8 +3298,11 @@
       <c r="AA10" s="8">
         <v>2602</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB10" s="8">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>4</v>
       </c>
@@ -3335,8 +3382,11 @@
       <c r="AA11" s="8">
         <v>2121</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB11" s="8">
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
@@ -3416,8 +3466,11 @@
       <c r="AA12" s="8">
         <v>774</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB12" s="8">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>8</v>
@@ -3494,6 +3547,9 @@
       </c>
       <c r="AA13" s="4">
         <v>33718</v>
+      </c>
+      <c r="AB13" s="4">
+        <v>38168</v>
       </c>
     </row>
   </sheetData>
@@ -3507,7 +3563,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA17"/>
+  <dimension ref="A1:AB17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
@@ -3521,42 +3577,42 @@
     <col min="3" max="20" width="10.7109375" customWidth="1"/>
     <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="24" width="10.7109375" style="23" customWidth="1"/>
-    <col min="25" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>325</v>
       </c>
       <c r="B3" s="11"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>333</v>
       </c>
       <c r="B4" s="11"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>328</v>
       </c>
       <c r="B5" s="11"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>327</v>
       </c>
       <c r="B6" s="11"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -3638,8 +3694,11 @@
       <c r="AA8" s="3">
         <v>43923</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB8" s="3">
+        <v>43924</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
@@ -3719,8 +3778,11 @@
       <c r="AA9" s="6">
         <v>1022</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB9" s="6">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
@@ -3802,8 +3864,11 @@
       <c r="AA10" s="8">
         <v>9291</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB10" s="29">
+        <v>10247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
@@ -3885,8 +3950,11 @@
       <c r="AA11" s="8">
         <v>3392</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB11" s="29">
+        <v>3732</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -3968,8 +4036,11 @@
       <c r="AA12" s="8">
         <v>1254</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB12" s="29">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
@@ -4051,8 +4122,11 @@
       <c r="AA13" s="8">
         <v>2233</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB13" s="29">
+        <v>2384</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
@@ -4134,8 +4208,11 @@
       <c r="AA14" s="8">
         <v>4694</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB14" s="29">
+        <v>5537</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
@@ -4217,8 +4294,11 @@
       <c r="AA15" s="8">
         <v>3269</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB15" s="29">
+        <v>3823</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>19</v>
       </c>
@@ -4300,8 +4380,11 @@
       <c r="AA16" s="8">
         <v>3066</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB16" s="29">
+        <v>3537</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -4382,6 +4465,9 @@
       </c>
       <c r="AA17" s="4">
         <v>28221</v>
+      </c>
+      <c r="AB17" s="4">
+        <v>31797</v>
       </c>
     </row>
   </sheetData>
@@ -4394,7 +4480,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB159"/>
+  <dimension ref="A1:AB160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
@@ -4409,7 +4495,7 @@
     <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="21" width="10.7109375" customWidth="1"/>
     <col min="22" max="24" width="10.7109375" style="23" customWidth="1"/>
-    <col min="25" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -4526,6 +4612,9 @@
       <c r="AA8" s="3">
         <v>43923</v>
       </c>
+      <c r="AB8" s="3">
+        <v>43924</v>
+      </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -4607,6 +4696,9 @@
       <c r="AA9" s="6">
         <v>1022</v>
       </c>
+      <c r="AB9" s="6">
+        <v>1151</v>
+      </c>
     </row>
     <row r="10" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -4690,7 +4782,9 @@
       <c r="AA10" s="8">
         <v>17</v>
       </c>
-      <c r="AB10" s="29"/>
+      <c r="AB10" s="8">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -4774,6 +4868,9 @@
       <c r="AA11" s="8">
         <v>74</v>
       </c>
+      <c r="AB11" s="8">
+        <v>92</v>
+      </c>
     </row>
     <row r="12" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -4857,6 +4954,9 @@
       <c r="AA12" s="8">
         <v>55</v>
       </c>
+      <c r="AB12" s="8">
+        <v>64</v>
+      </c>
     </row>
     <row r="13" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -4940,6 +5040,9 @@
       <c r="AA13" s="8">
         <v>70</v>
       </c>
+      <c r="AB13" s="8">
+        <v>77</v>
+      </c>
     </row>
     <row r="14" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -5023,6 +5126,9 @@
       <c r="AA14" s="8">
         <v>30</v>
       </c>
+      <c r="AB14" s="8">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -5106,6 +5212,9 @@
       <c r="AA15" s="8">
         <v>41</v>
       </c>
+      <c r="AB15" s="8">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -5189,8 +5298,11 @@
       <c r="AA16" s="8">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB16" s="8">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>304</v>
       </c>
@@ -5272,8 +5384,11 @@
       <c r="AA17" s="8">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB17" s="8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>282</v>
       </c>
@@ -5355,8 +5470,11 @@
       <c r="AA18" s="8">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB18" s="8">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>308</v>
       </c>
@@ -5438,8 +5556,11 @@
       <c r="AA19" s="8">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB19" s="8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>180</v>
       </c>
@@ -5521,8 +5642,11 @@
       <c r="AA20" s="8">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB20" s="8">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>318</v>
       </c>
@@ -5604,8 +5728,11 @@
       <c r="AA21" s="8">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB21" s="8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>310</v>
       </c>
@@ -5687,8 +5814,11 @@
       <c r="AA22" s="8">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB22" s="8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>244</v>
       </c>
@@ -5770,8 +5900,11 @@
       <c r="AA23" s="8">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB23" s="8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>196</v>
       </c>
@@ -5853,8 +5986,11 @@
       <c r="AA24" s="8">
         <v>167</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB24" s="8">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>238</v>
       </c>
@@ -5936,8 +6072,11 @@
       <c r="AA25" s="8">
         <v>107</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB25" s="8">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>320</v>
       </c>
@@ -6019,8 +6158,11 @@
       <c r="AA26" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB26" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>144</v>
       </c>
@@ -6102,8 +6244,11 @@
       <c r="AA27" s="8">
         <v>125</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB27" s="8">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>274</v>
       </c>
@@ -6185,8 +6330,11 @@
       <c r="AA28" s="8">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB28" s="8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>322</v>
       </c>
@@ -6268,8 +6416,11 @@
       <c r="AA29" s="8">
         <v>51</v>
       </c>
-    </row>
-    <row r="30" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB29" s="8">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>288</v>
       </c>
@@ -6351,8 +6502,11 @@
       <c r="AA30" s="8">
         <v>61</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB30" s="8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>246</v>
       </c>
@@ -6434,8 +6588,11 @@
       <c r="AA31" s="8">
         <v>52</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB31" s="8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>166</v>
       </c>
@@ -6517,8 +6674,11 @@
       <c r="AA32" s="8">
         <v>137</v>
       </c>
-    </row>
-    <row r="33" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB32" s="8">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>256</v>
       </c>
@@ -6600,8 +6760,11 @@
       <c r="AA33" s="8">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB33" s="8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>160</v>
       </c>
@@ -6683,8 +6846,11 @@
       <c r="AA34" s="8">
         <v>91</v>
       </c>
-    </row>
-    <row r="35" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB34" s="8">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>216</v>
       </c>
@@ -6766,8 +6932,11 @@
       <c r="AA35" s="8">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB35" s="8">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>202</v>
       </c>
@@ -6849,8 +7018,11 @@
       <c r="AA36" s="8">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB36" s="8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>250</v>
       </c>
@@ -6932,8 +7104,11 @@
       <c r="AA37" s="8">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB37" s="8">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>294</v>
       </c>
@@ -7015,8 +7190,11 @@
       <c r="AA38" s="8">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB38" s="8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>276</v>
       </c>
@@ -7098,8 +7276,11 @@
       <c r="AA39" s="8">
         <v>115</v>
       </c>
-    </row>
-    <row r="40" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB39" s="8">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>262</v>
       </c>
@@ -7181,8 +7362,11 @@
       <c r="AA40" s="8">
         <v>71</v>
       </c>
-    </row>
-    <row r="41" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB40" s="8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>268</v>
       </c>
@@ -7264,8 +7448,11 @@
       <c r="AA41" s="8">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB41" s="8">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>198</v>
       </c>
@@ -7347,8 +7534,11 @@
       <c r="AA42" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="43" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB42" s="8">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>270</v>
       </c>
@@ -7430,8 +7620,11 @@
       <c r="AA43" s="8">
         <v>36</v>
       </c>
-    </row>
-    <row r="44" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB43" s="8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>280</v>
       </c>
@@ -7513,8 +7706,11 @@
       <c r="AA44" s="8">
         <v>66</v>
       </c>
-    </row>
-    <row r="45" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB44" s="8">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>218</v>
       </c>
@@ -7596,8 +7792,11 @@
       <c r="AA45" s="8">
         <v>67</v>
       </c>
-    </row>
-    <row r="46" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB45" s="8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>116</v>
       </c>
@@ -7679,8 +7878,11 @@
       <c r="AA46" s="8">
         <v>117</v>
       </c>
-    </row>
-    <row r="47" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB46" s="8">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>150</v>
       </c>
@@ -7762,8 +7964,11 @@
       <c r="AA47" s="8">
         <v>75</v>
       </c>
-    </row>
-    <row r="48" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB47" s="8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>194</v>
       </c>
@@ -7845,8 +8050,11 @@
       <c r="AA48" s="8">
         <v>67</v>
       </c>
-    </row>
-    <row r="49" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB48" s="8">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>240</v>
       </c>
@@ -7928,8 +8136,11 @@
       <c r="AA49" s="8">
         <v>127</v>
       </c>
-    </row>
-    <row r="50" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB49" s="8">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>164</v>
       </c>
@@ -8011,8 +8222,11 @@
       <c r="AA50" s="8">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB50" s="8">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>242</v>
       </c>
@@ -8094,8 +8308,11 @@
       <c r="AA51" s="8">
         <v>83</v>
       </c>
-    </row>
-    <row r="52" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB51" s="8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>210</v>
       </c>
@@ -8177,8 +8394,11 @@
       <c r="AA52" s="8">
         <v>105</v>
       </c>
-    </row>
-    <row r="53" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB52" s="8">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>292</v>
       </c>
@@ -8260,8 +8480,11 @@
       <c r="AA53" s="8">
         <v>17</v>
       </c>
-    </row>
-    <row r="54" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB53" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>236</v>
       </c>
@@ -8343,8 +8566,11 @@
       <c r="AA54" s="8">
         <v>165</v>
       </c>
-    </row>
-    <row r="55" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB54" s="8">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>192</v>
       </c>
@@ -8426,8 +8652,11 @@
       <c r="AA55" s="8">
         <v>102</v>
       </c>
-    </row>
-    <row r="56" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB55" s="8">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>212</v>
       </c>
@@ -8509,8 +8738,11 @@
       <c r="AA56" s="8">
         <v>97</v>
       </c>
-    </row>
-    <row r="57" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB56" s="8">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>278</v>
       </c>
@@ -8592,8 +8824,11 @@
       <c r="AA57" s="8">
         <v>106</v>
       </c>
-    </row>
-    <row r="58" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB57" s="8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>178</v>
       </c>
@@ -8675,8 +8910,11 @@
       <c r="AA58" s="8">
         <v>114</v>
       </c>
-    </row>
-    <row r="59" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB58" s="8">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>162</v>
       </c>
@@ -8758,8 +8996,11 @@
       <c r="AA59" s="8">
         <v>105</v>
       </c>
-    </row>
-    <row r="60" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB59" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>302</v>
       </c>
@@ -8841,8 +9082,11 @@
       <c r="AA60" s="8">
         <v>72</v>
       </c>
-    </row>
-    <row r="61" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB60" s="8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>222</v>
       </c>
@@ -8924,8 +9168,11 @@
       <c r="AA61" s="8">
         <v>99</v>
       </c>
-    </row>
-    <row r="62" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB61" s="8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>230</v>
       </c>
@@ -9007,8 +9254,11 @@
       <c r="AA62" s="8">
         <v>119</v>
       </c>
-    </row>
-    <row r="63" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB62" s="8">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>190</v>
       </c>
@@ -9090,8 +9340,11 @@
       <c r="AA63" s="8">
         <v>58</v>
       </c>
-    </row>
-    <row r="64" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB63" s="8">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>214</v>
       </c>
@@ -9173,8 +9426,11 @@
       <c r="AA64" s="8">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB64" s="8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>188</v>
       </c>
@@ -9256,8 +9512,11 @@
       <c r="AA65" s="8">
         <v>69</v>
       </c>
-    </row>
-    <row r="66" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB65" s="8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>204</v>
       </c>
@@ -9339,8 +9598,11 @@
       <c r="AA66" s="8">
         <v>87</v>
       </c>
-    </row>
-    <row r="67" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB66" s="8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>106</v>
       </c>
@@ -9422,8 +9684,11 @@
       <c r="AA67" s="8">
         <v>195</v>
       </c>
-    </row>
-    <row r="68" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB67" s="8">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="68" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>138</v>
       </c>
@@ -9505,8 +9770,11 @@
       <c r="AA68" s="8">
         <v>125</v>
       </c>
-    </row>
-    <row r="69" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB68" s="8">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>184</v>
       </c>
@@ -9588,8 +9856,11 @@
       <c r="AA69" s="8">
         <v>105</v>
       </c>
-    </row>
-    <row r="70" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB69" s="8">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>182</v>
       </c>
@@ -9671,8 +9942,11 @@
       <c r="AA70" s="8">
         <v>158</v>
       </c>
-    </row>
-    <row r="71" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB70" s="8">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="71" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>146</v>
       </c>
@@ -9754,8 +10028,11 @@
       <c r="AA71" s="8">
         <v>140</v>
       </c>
-    </row>
-    <row r="72" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB71" s="8">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="72" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>142</v>
       </c>
@@ -9837,8 +10114,11 @@
       <c r="AA72" s="8">
         <v>94</v>
       </c>
-    </row>
-    <row r="73" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB72" s="8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>156</v>
       </c>
@@ -9920,8 +10200,11 @@
       <c r="AA73" s="8">
         <v>126</v>
       </c>
-    </row>
-    <row r="74" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB73" s="8">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>260</v>
       </c>
@@ -10003,8 +10286,11 @@
       <c r="AA74" s="8">
         <v>91</v>
       </c>
-    </row>
-    <row r="75" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB74" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>264</v>
       </c>
@@ -10086,8 +10372,11 @@
       <c r="AA75" s="8">
         <v>79</v>
       </c>
-    </row>
-    <row r="76" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB75" s="8">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="76" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>154</v>
       </c>
@@ -10169,8 +10458,11 @@
       <c r="AA76" s="8">
         <v>309</v>
       </c>
-    </row>
-    <row r="77" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB76" s="8">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="77" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>298</v>
       </c>
@@ -10252,8 +10544,11 @@
       <c r="AA77" s="8">
         <v>112</v>
       </c>
-    </row>
-    <row r="78" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB77" s="8">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>232</v>
       </c>
@@ -10335,8 +10630,11 @@
       <c r="AA78" s="8">
         <v>119</v>
       </c>
-    </row>
-    <row r="79" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB78" s="8">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="79" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>208</v>
       </c>
@@ -10418,8 +10716,11 @@
       <c r="AA79" s="8">
         <v>111</v>
       </c>
-    </row>
-    <row r="80" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB79" s="8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="80" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>220</v>
       </c>
@@ -10501,8 +10802,11 @@
       <c r="AA80" s="8">
         <v>134</v>
       </c>
-    </row>
-    <row r="81" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB80" s="8">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>300</v>
       </c>
@@ -10584,8 +10888,11 @@
       <c r="AA81" s="8">
         <v>95</v>
       </c>
-    </row>
-    <row r="82" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB81" s="8">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>284</v>
       </c>
@@ -10667,8 +10974,11 @@
       <c r="AA82" s="8">
         <v>129</v>
       </c>
-    </row>
-    <row r="83" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB82" s="8">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>54</v>
       </c>
@@ -10750,8 +11060,11 @@
       <c r="AA83" s="8">
         <v>602</v>
       </c>
-    </row>
-    <row r="84" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB83" s="8">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>108</v>
       </c>
@@ -10833,8 +11146,11 @@
       <c r="AA84" s="8">
         <v>252</v>
       </c>
-    </row>
-    <row r="85" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB84" s="8">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>174</v>
       </c>
@@ -10916,8 +11232,11 @@
       <c r="AA85" s="8">
         <v>113</v>
       </c>
-    </row>
-    <row r="86" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB85" s="8">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>296</v>
       </c>
@@ -10999,8 +11318,11 @@
       <c r="AA86" s="8">
         <v>53</v>
       </c>
-    </row>
-    <row r="87" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB86" s="8">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>248</v>
       </c>
@@ -11082,8 +11404,11 @@
       <c r="AA87" s="8">
         <v>131</v>
       </c>
-    </row>
-    <row r="88" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB87" s="8">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>68</v>
       </c>
@@ -11165,8 +11490,11 @@
       <c r="AA88" s="8">
         <v>852</v>
       </c>
-    </row>
-    <row r="89" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB88" s="8">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>252</v>
       </c>
@@ -11248,8 +11576,11 @@
       <c r="AA89" s="8">
         <v>155</v>
       </c>
-    </row>
-    <row r="90" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB89" s="8">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="90" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>170</v>
       </c>
@@ -11331,8 +11662,11 @@
       <c r="AA90" s="8">
         <v>194</v>
       </c>
-    </row>
-    <row r="91" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB90" s="8">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>224</v>
       </c>
@@ -11414,8 +11748,11 @@
       <c r="AA91" s="8">
         <v>215</v>
       </c>
-    </row>
-    <row r="92" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB91" s="8">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="92" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>314</v>
       </c>
@@ -11497,8 +11834,11 @@
       <c r="AA92" s="8">
         <v>141</v>
       </c>
-    </row>
-    <row r="93" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB92" s="8">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="93" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>124</v>
       </c>
@@ -11580,8 +11920,11 @@
       <c r="AA93" s="8">
         <v>231</v>
       </c>
-    </row>
-    <row r="94" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB93" s="8">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>92</v>
       </c>
@@ -11663,8 +12006,11 @@
       <c r="AA94" s="8">
         <v>222</v>
       </c>
-    </row>
-    <row r="95" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB94" s="8">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>228</v>
       </c>
@@ -11746,8 +12092,11 @@
       <c r="AA95" s="8">
         <v>118</v>
       </c>
-    </row>
-    <row r="96" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB95" s="8">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="96" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>272</v>
       </c>
@@ -11829,8 +12178,11 @@
       <c r="AA96" s="8">
         <v>60</v>
       </c>
-    </row>
-    <row r="97" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB96" s="8">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>266</v>
       </c>
@@ -11912,8 +12264,11 @@
       <c r="AA97" s="8">
         <v>114</v>
       </c>
-    </row>
-    <row r="98" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB97" s="8">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="98" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>130</v>
       </c>
@@ -11995,8 +12350,11 @@
       <c r="AA98" s="8">
         <v>203</v>
       </c>
-    </row>
-    <row r="99" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB98" s="8">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="99" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>234</v>
       </c>
@@ -12078,8 +12436,11 @@
       <c r="AA99" s="8">
         <v>95</v>
       </c>
-    </row>
-    <row r="100" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB99" s="8">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>306</v>
       </c>
@@ -12161,8 +12522,11 @@
       <c r="AA100" s="8">
         <v>95</v>
       </c>
-    </row>
-    <row r="101" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB100" s="8">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="101" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>112</v>
       </c>
@@ -12244,8 +12608,11 @@
       <c r="AA101" s="8">
         <v>141</v>
       </c>
-    </row>
-    <row r="102" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB101" s="8">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="102" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>96</v>
       </c>
@@ -12327,8 +12694,11 @@
       <c r="AA102" s="8">
         <v>510</v>
       </c>
-    </row>
-    <row r="103" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB102" s="8">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="103" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>104</v>
       </c>
@@ -12410,8 +12780,11 @@
       <c r="AA103" s="8">
         <v>190</v>
       </c>
-    </row>
-    <row r="104" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB103" s="8">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="104" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>36</v>
       </c>
@@ -12493,8 +12866,11 @@
       <c r="AA104" s="8">
         <v>559</v>
       </c>
-    </row>
-    <row r="105" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB104" s="8">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="105" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>52</v>
       </c>
@@ -12576,8 +12952,11 @@
       <c r="AA105" s="8">
         <v>366</v>
       </c>
-    </row>
-    <row r="106" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB105" s="8">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="106" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>64</v>
       </c>
@@ -12659,8 +13038,11 @@
       <c r="AA106" s="8">
         <v>225</v>
       </c>
-    </row>
-    <row r="107" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB106" s="8">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="107" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>46</v>
       </c>
@@ -12742,8 +13124,11 @@
       <c r="AA107" s="8">
         <v>437</v>
       </c>
-    </row>
-    <row r="108" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB107" s="8">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="108" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>42</v>
       </c>
@@ -12825,8 +13210,11 @@
       <c r="AA108" s="8">
         <v>385</v>
       </c>
-    </row>
-    <row r="109" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB108" s="8">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="109" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>84</v>
       </c>
@@ -12908,8 +13296,11 @@
       <c r="AA109" s="8">
         <v>264</v>
       </c>
-    </row>
-    <row r="110" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB109" s="8">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="110" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>72</v>
       </c>
@@ -12991,8 +13382,11 @@
       <c r="AA110" s="8">
         <v>247</v>
       </c>
-    </row>
-    <row r="111" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB110" s="8">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="111" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>78</v>
       </c>
@@ -13074,8 +13468,11 @@
       <c r="AA111" s="8">
         <v>266</v>
       </c>
-    </row>
-    <row r="112" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB111" s="8">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="112" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>94</v>
       </c>
@@ -13157,8 +13554,11 @@
       <c r="AA112" s="8">
         <v>188</v>
       </c>
-    </row>
-    <row r="113" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB112" s="8">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="113" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>80</v>
       </c>
@@ -13240,8 +13640,11 @@
       <c r="AA113" s="8">
         <v>211</v>
       </c>
-    </row>
-    <row r="114" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB113" s="8">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="114" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>40</v>
       </c>
@@ -13323,8 +13726,11 @@
       <c r="AA114" s="8">
         <v>378</v>
       </c>
-    </row>
-    <row r="115" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB114" s="8">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="115" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>134</v>
       </c>
@@ -13406,8 +13812,11 @@
       <c r="AA115" s="8">
         <v>142</v>
       </c>
-    </row>
-    <row r="116" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB115" s="8">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="116" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>86</v>
       </c>
@@ -13489,8 +13898,11 @@
       <c r="AA116" s="8">
         <v>250</v>
       </c>
-    </row>
-    <row r="117" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB116" s="8">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="117" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>88</v>
       </c>
@@ -13572,8 +13984,11 @@
       <c r="AA117" s="8">
         <v>234</v>
       </c>
-    </row>
-    <row r="118" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB117" s="8">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="118" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>66</v>
       </c>
@@ -13655,8 +14070,11 @@
       <c r="AA118" s="8">
         <v>188</v>
       </c>
-    </row>
-    <row r="119" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB118" s="8">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="119" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>38</v>
       </c>
@@ -13738,8 +14156,11 @@
       <c r="AA119" s="8">
         <v>208</v>
       </c>
-    </row>
-    <row r="120" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB119" s="8">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="120" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>136</v>
       </c>
@@ -13821,8 +14242,11 @@
       <c r="AA120" s="8">
         <v>127</v>
       </c>
-    </row>
-    <row r="121" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB120" s="8">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="121" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>30</v>
       </c>
@@ -13904,8 +14328,11 @@
       <c r="AA121" s="8">
         <v>508</v>
       </c>
-    </row>
-    <row r="122" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB121" s="8">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="122" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>56</v>
       </c>
@@ -13987,8 +14414,11 @@
       <c r="AA122" s="8">
         <v>346</v>
       </c>
-    </row>
-    <row r="123" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB122" s="8">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="123" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>60</v>
       </c>
@@ -14070,8 +14500,11 @@
       <c r="AA123" s="8">
         <v>235</v>
       </c>
-    </row>
-    <row r="124" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB123" s="8">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="124" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>76</v>
       </c>
@@ -14153,8 +14586,11 @@
       <c r="AA124" s="8">
         <v>370</v>
       </c>
-    </row>
-    <row r="125" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB124" s="8">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="125" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>110</v>
       </c>
@@ -14236,8 +14672,11 @@
       <c r="AA125" s="8">
         <v>212</v>
       </c>
-    </row>
-    <row r="126" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB125" s="8">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="126" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>158</v>
       </c>
@@ -14319,8 +14758,11 @@
       <c r="AA126" s="8">
         <v>155</v>
       </c>
-    </row>
-    <row r="127" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB126" s="8">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="127" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>28</v>
       </c>
@@ -14402,8 +14844,11 @@
       <c r="AA127" s="8">
         <v>516</v>
       </c>
-    </row>
-    <row r="128" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB127" s="8">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="128" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>140</v>
       </c>
@@ -14485,8 +14930,11 @@
       <c r="AA128" s="8">
         <v>176</v>
       </c>
-    </row>
-    <row r="129" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB128" s="8">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="129" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
         <v>74</v>
       </c>
@@ -14568,8 +15016,11 @@
       <c r="AA129" s="8">
         <v>259</v>
       </c>
-    </row>
-    <row r="130" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB129" s="8">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="130" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>120</v>
       </c>
@@ -14651,8 +15102,11 @@
       <c r="AA130" s="8">
         <v>290</v>
       </c>
-    </row>
-    <row r="131" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB130" s="8">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="131" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>34</v>
       </c>
@@ -14734,8 +15188,11 @@
       <c r="AA131" s="8">
         <v>397</v>
       </c>
-    </row>
-    <row r="132" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB131" s="8">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="132" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>32</v>
       </c>
@@ -14817,8 +15274,11 @@
       <c r="AA132" s="8">
         <v>311</v>
       </c>
-    </row>
-    <row r="133" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB132" s="8">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="133" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
         <v>58</v>
       </c>
@@ -14900,8 +15360,11 @@
       <c r="AA133" s="8">
         <v>212</v>
       </c>
-    </row>
-    <row r="134" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB133" s="8">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="134" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>132</v>
       </c>
@@ -14983,8 +15446,11 @@
       <c r="AA134" s="8">
         <v>166</v>
       </c>
-    </row>
-    <row r="135" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB134" s="8">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="135" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
         <v>62</v>
       </c>
@@ -15066,8 +15532,11 @@
       <c r="AA135" s="8">
         <v>512</v>
       </c>
-    </row>
-    <row r="136" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB135" s="8">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="136" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
         <v>50</v>
       </c>
@@ -15149,8 +15618,11 @@
       <c r="AA136" s="8">
         <v>342</v>
       </c>
-    </row>
-    <row r="137" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB136" s="8">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="137" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
         <v>98</v>
       </c>
@@ -15232,8 +15704,11 @@
       <c r="AA137" s="8">
         <v>147</v>
       </c>
-    </row>
-    <row r="138" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB137" s="8">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="138" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
         <v>206</v>
       </c>
@@ -15315,8 +15790,11 @@
       <c r="AA138" s="8">
         <v>95</v>
       </c>
-    </row>
-    <row r="139" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB138" s="8">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="139" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>82</v>
       </c>
@@ -15398,8 +15876,11 @@
       <c r="AA139" s="8">
         <v>517</v>
       </c>
-    </row>
-    <row r="140" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB139" s="8">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="140" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
         <v>128</v>
       </c>
@@ -15481,8 +15962,11 @@
       <c r="AA140" s="8">
         <v>208</v>
       </c>
-    </row>
-    <row r="141" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB140" s="8">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="141" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
         <v>26</v>
       </c>
@@ -15564,8 +16048,11 @@
       <c r="AA141" s="8">
         <v>699</v>
       </c>
-    </row>
-    <row r="142" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB141" s="8">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="142" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
         <v>44</v>
       </c>
@@ -15647,8 +16134,11 @@
       <c r="AA142" s="8">
         <v>582</v>
       </c>
-    </row>
-    <row r="143" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB142" s="8">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="143" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
         <v>100</v>
       </c>
@@ -15730,8 +16220,11 @@
       <c r="AA143" s="8">
         <v>531</v>
       </c>
-    </row>
-    <row r="144" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB143" s="8">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="144" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
         <v>102</v>
       </c>
@@ -15813,8 +16306,11 @@
       <c r="AA144" s="8">
         <v>463</v>
       </c>
-    </row>
-    <row r="145" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB144" s="8">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="145" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
         <v>118</v>
       </c>
@@ -15896,8 +16392,11 @@
       <c r="AA145" s="8">
         <v>201</v>
       </c>
-    </row>
-    <row r="146" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB145" s="8">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="146" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
         <v>226</v>
       </c>
@@ -15979,8 +16478,11 @@
       <c r="AA146" s="8">
         <v>153</v>
       </c>
-    </row>
-    <row r="147" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB146" s="8">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="147" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
         <v>168</v>
       </c>
@@ -16062,8 +16564,11 @@
       <c r="AA147" s="8">
         <v>207</v>
       </c>
-    </row>
-    <row r="148" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB147" s="8">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="148" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
         <v>126</v>
       </c>
@@ -16145,8 +16650,11 @@
       <c r="AA148" s="8">
         <v>220</v>
       </c>
-    </row>
-    <row r="149" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB148" s="8">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="149" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>152</v>
       </c>
@@ -16228,8 +16736,11 @@
       <c r="AA149" s="8">
         <v>163</v>
       </c>
-    </row>
-    <row r="150" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB149" s="8">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="150" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
         <v>90</v>
       </c>
@@ -16311,8 +16822,11 @@
       <c r="AA150" s="8">
         <v>298</v>
       </c>
-    </row>
-    <row r="151" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB150" s="8">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="151" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
         <v>70</v>
       </c>
@@ -16394,8 +16908,11 @@
       <c r="AA151" s="8">
         <v>277</v>
       </c>
-    </row>
-    <row r="152" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB151" s="8">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="152" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>176</v>
       </c>
@@ -16477,8 +16994,11 @@
       <c r="AA152" s="8">
         <v>68</v>
       </c>
-    </row>
-    <row r="153" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB152" s="8">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="153" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
         <v>114</v>
       </c>
@@ -16560,8 +17080,11 @@
       <c r="AA153" s="8">
         <v>372</v>
       </c>
-    </row>
-    <row r="154" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB153" s="8">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="154" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
         <v>148</v>
       </c>
@@ -16643,8 +17166,11 @@
       <c r="AA154" s="8">
         <v>157</v>
       </c>
-    </row>
-    <row r="155" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB154" s="8">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="155" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
         <v>48</v>
       </c>
@@ -16726,8 +17252,11 @@
       <c r="AA155" s="8">
         <v>618</v>
       </c>
-    </row>
-    <row r="156" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB155" s="8">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="156" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
         <v>172</v>
       </c>
@@ -16809,8 +17338,11 @@
       <c r="AA156" s="8">
         <v>235</v>
       </c>
-    </row>
-    <row r="157" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB156" s="8">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="157" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
         <v>122</v>
       </c>
@@ -16892,8 +17424,11 @@
       <c r="AA157" s="8">
         <v>172</v>
       </c>
-    </row>
-    <row r="158" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AB157" s="8">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="158" spans="1:28" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
         <v>200</v>
       </c>
@@ -16975,8 +17510,11 @@
       <c r="AA158" s="8">
         <v>221</v>
       </c>
-    </row>
-    <row r="159" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB158" s="8">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="159" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>0</v>
       </c>
@@ -17058,6 +17596,12 @@
       <c r="AA159" s="4">
         <v>28221</v>
       </c>
+      <c r="AB159" s="4">
+        <v>31797</v>
+      </c>
+    </row>
+    <row r="160" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AB160" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>